<commit_message>
added resource for maternal parity
</commit_message>
<xml_diff>
--- a/output/observations-summary.xlsx
+++ b/output/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Profile</t>
   </si>
@@ -45,6 +45,27 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>mh-toc-parity</t>
+  </si>
+  <si>
+    <t>MH TOC Parity Profile</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>LOINC#11977-6</t>
+  </si>
+  <si>
+    <t>dateTimeĵ, Periodĵ, Timingĵ, instantĵ</t>
+  </si>
+  <si>
+    <t>integerĵ, timeĵ, dateTimeĵ, Periodĵ</t>
+  </si>
+  <si>
+    <t>optional</t>
   </si>
 </sst>
 </file>
@@ -178,7 +199,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -219,6 +240,41 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>